<commit_message>
Clustering of categories successful
</commit_message>
<xml_diff>
--- a/DataVisualization.xlsx
+++ b/DataVisualization.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chakotay Incorvaia\dev2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5B6332A-FCD0-4CB0-B7B5-124B3A4D4D02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60C5F49D-9523-48ED-A63A-86E5A38D3636}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{CCE0E44F-0ABA-4097-A493-E6A10D57D926}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Accuracy</t>
   </si>
@@ -77,9 +77,6 @@
     <t>Engine Display</t>
   </si>
   <si>
-    <t>Ice and Rain Protective Panels</t>
-  </si>
-  <si>
     <t>Fuel Panel</t>
   </si>
   <si>
@@ -89,22 +86,13 @@
     <t>Flight Controls Panel</t>
   </si>
   <si>
-    <t>Crew Commnications</t>
-  </si>
-  <si>
     <t>TCAS Transponder</t>
   </si>
   <si>
     <t>Navigational Radio</t>
   </si>
   <si>
-    <t>Radio Tuning Panel</t>
-  </si>
-  <si>
     <t>Audio Control Panel</t>
-  </si>
-  <si>
-    <t>Auxiliary Power Unit</t>
   </si>
   <si>
     <t>Cabin Pressurization Panel</t>
@@ -527,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49A2CE25-1FB0-46F3-A95B-A7BCC2B1E34D}">
-  <dimension ref="A1:AB27"/>
+  <dimension ref="A1:X27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="L41" sqref="L41"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,90 +532,74 @@
     <col min="7" max="7" width="19.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="27.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="30.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="18.28515625" style="2" customWidth="1"/>
-    <col min="23" max="23" width="17.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="19.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="20.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="19.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="14.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="28" max="16384" width="9.140625" style="2"/>
+    <col min="10" max="10" width="20.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.28515625" style="2" customWidth="1"/>
+    <col min="19" max="19" width="17.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="20.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="T1" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -659,10 +631,10 @@
         <v>4</v>
       </c>
       <c r="K2" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L2" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M2" s="3">
         <v>5</v>
@@ -671,202 +643,166 @@
         <v>5</v>
       </c>
       <c r="O2" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P2" s="3">
-        <v>5</v>
-      </c>
-      <c r="Q2" s="3">
-        <v>5</v>
-      </c>
-      <c r="R2" s="3">
-        <v>4</v>
-      </c>
-      <c r="S2" s="3">
-        <v>4</v>
-      </c>
-      <c r="T2" s="3">
-        <v>4</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
       <c r="U2" s="3"/>
       <c r="V2" s="3"/>
       <c r="W2" s="3"/>
-      <c r="X2" s="3"/>
-      <c r="Y2" s="3"/>
-      <c r="Z2" s="3"/>
-      <c r="AA2" s="3"/>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B3" s="2">
-        <v>5</v>
-      </c>
-      <c r="C3" s="2">
-        <v>5</v>
-      </c>
-      <c r="D3" s="2">
-        <v>5</v>
+        <v>31</v>
+      </c>
+      <c r="B3" s="3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3">
+        <v>3</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1</v>
       </c>
       <c r="E3" s="3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F3" s="3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G3" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H3" s="3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I3" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J3" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K3" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L3" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M3" s="3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="N3" s="3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="O3" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="P3" s="3">
-        <v>4</v>
-      </c>
-      <c r="Q3" s="3">
-        <v>3</v>
-      </c>
-      <c r="R3" s="3">
-        <v>5</v>
-      </c>
-      <c r="S3" s="3">
-        <v>4</v>
-      </c>
-      <c r="T3" s="3">
-        <v>4</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
       <c r="U3" s="3"/>
       <c r="V3" s="3"/>
       <c r="W3" s="3"/>
-      <c r="X3" s="3"/>
-      <c r="Y3" s="3"/>
-      <c r="Z3" s="3"/>
-      <c r="AA3" s="3"/>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>1</v>
+        <v>41</v>
       </c>
       <c r="B4" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C4" s="2">
         <v>5</v>
       </c>
       <c r="D4" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E4" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F4" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G4" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H4" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I4" s="3">
         <v>4</v>
       </c>
       <c r="J4" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K4" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="L4" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M4" s="3">
         <v>4</v>
       </c>
       <c r="N4" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="O4" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P4" s="3">
         <v>4</v>
       </c>
-      <c r="Q4" s="3">
-        <v>4</v>
-      </c>
-      <c r="R4" s="3">
-        <v>4</v>
-      </c>
-      <c r="S4" s="3">
-        <v>3</v>
-      </c>
-      <c r="T4" s="3">
-        <v>4</v>
-      </c>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
       <c r="U4" s="3"/>
       <c r="V4" s="3"/>
       <c r="W4" s="3"/>
-      <c r="X4" s="3"/>
-      <c r="Y4" s="3"/>
-      <c r="Z4" s="3"/>
-      <c r="AA4" s="3"/>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" s="3">
-        <v>5</v>
-      </c>
-      <c r="C5" s="3">
-        <v>5</v>
-      </c>
-      <c r="D5" s="3">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2">
+        <v>4</v>
+      </c>
+      <c r="C5" s="2">
+        <v>5</v>
+      </c>
+      <c r="D5" s="2">
         <v>4</v>
       </c>
       <c r="E5" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F5" s="3">
         <v>4</v>
       </c>
       <c r="G5" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H5" s="3">
         <v>4</v>
       </c>
       <c r="I5" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J5" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K5" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L5" s="3">
         <v>5</v>
@@ -878,172 +814,136 @@
         <v>4</v>
       </c>
       <c r="O5" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P5" s="3">
         <v>4</v>
       </c>
-      <c r="Q5" s="3">
-        <v>5</v>
-      </c>
-      <c r="R5" s="3">
-        <v>5</v>
-      </c>
-      <c r="S5" s="3">
-        <v>4</v>
-      </c>
-      <c r="T5" s="3">
-        <v>5</v>
-      </c>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
       <c r="U5" s="3"/>
       <c r="V5" s="3"/>
       <c r="W5" s="3"/>
-      <c r="X5" s="3"/>
-      <c r="Y5" s="3"/>
-      <c r="Z5" s="3"/>
-      <c r="AA5" s="3"/>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B6" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C6" s="3">
         <v>5</v>
       </c>
       <c r="D6" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E6" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F6" s="3">
         <v>4</v>
       </c>
       <c r="G6" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H6" s="3">
         <v>4</v>
       </c>
       <c r="I6" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J6" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="K6" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L6" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M6" s="3">
         <v>4</v>
       </c>
       <c r="N6" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O6" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="P6" s="3">
-        <v>4</v>
-      </c>
-      <c r="Q6" s="3">
-        <v>4</v>
-      </c>
-      <c r="R6" s="3">
-        <v>4</v>
-      </c>
-      <c r="S6" s="3">
-        <v>3</v>
-      </c>
-      <c r="T6" s="3">
-        <v>4</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
       <c r="U6" s="3"/>
       <c r="V6" s="3"/>
       <c r="W6" s="3"/>
-      <c r="X6" s="3"/>
-      <c r="Y6" s="3"/>
-      <c r="Z6" s="3"/>
-      <c r="AA6" s="3"/>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B7" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C7" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D7" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E7" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F7" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G7" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H7" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I7" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J7" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K7" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="L7" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="M7" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="N7" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="O7" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="P7" s="3">
-        <v>1</v>
-      </c>
-      <c r="Q7" s="3">
-        <v>1</v>
-      </c>
-      <c r="R7" s="3">
-        <v>1</v>
-      </c>
-      <c r="S7" s="3">
-        <v>1</v>
-      </c>
-      <c r="T7" s="3">
-        <v>1</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="3"/>
       <c r="U7" s="3"/>
       <c r="V7" s="3"/>
       <c r="W7" s="3"/>
-      <c r="X7" s="3"/>
-      <c r="Y7" s="3"/>
-      <c r="Z7" s="3"/>
-      <c r="AA7" s="3"/>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B8" s="3">
         <v>4</v>
@@ -1070,19 +970,19 @@
         <v>4</v>
       </c>
       <c r="J8" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K8" s="3">
         <v>4</v>
       </c>
       <c r="L8" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M8" s="3">
         <v>4</v>
       </c>
       <c r="N8" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O8" s="3">
         <v>4</v>
@@ -1090,27 +990,15 @@
       <c r="P8" s="3">
         <v>4</v>
       </c>
-      <c r="Q8" s="3">
-        <v>3</v>
-      </c>
-      <c r="R8" s="3">
-        <v>4</v>
-      </c>
-      <c r="S8" s="3">
-        <v>3</v>
-      </c>
-      <c r="T8" s="3">
-        <v>4</v>
-      </c>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
+      <c r="T8" s="3"/>
       <c r="U8" s="3"/>
       <c r="V8" s="3"/>
       <c r="W8" s="3"/>
-      <c r="X8" s="3"/>
-      <c r="Y8" s="3"/>
-      <c r="Z8" s="3"/>
-      <c r="AA8" s="3"/>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
@@ -1142,44 +1030,32 @@
         <v>4</v>
       </c>
       <c r="K9" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L9" s="3">
         <v>4</v>
       </c>
       <c r="M9" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N9" s="3">
         <v>4</v>
       </c>
       <c r="O9" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P9" s="3">
         <v>4</v>
       </c>
-      <c r="Q9" s="3">
-        <v>4</v>
-      </c>
-      <c r="R9" s="3">
-        <v>4</v>
-      </c>
-      <c r="S9" s="3">
-        <v>2</v>
-      </c>
-      <c r="T9" s="3">
-        <v>4</v>
-      </c>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
+      <c r="T9" s="3"/>
       <c r="U9" s="3"/>
       <c r="V9" s="3"/>
       <c r="W9" s="3"/>
-      <c r="X9" s="3"/>
-      <c r="Y9" s="3"/>
-      <c r="Z9" s="3"/>
-      <c r="AA9" s="3"/>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>3</v>
       </c>
@@ -1208,7 +1084,7 @@
         <v>4</v>
       </c>
       <c r="J10" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K10" s="3">
         <v>4</v>
@@ -1220,37 +1096,25 @@
         <v>4</v>
       </c>
       <c r="N10" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O10" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="P10" s="3">
-        <v>4</v>
-      </c>
-      <c r="Q10" s="3">
-        <v>5</v>
-      </c>
-      <c r="R10" s="3">
-        <v>4</v>
-      </c>
-      <c r="S10" s="3">
-        <v>2</v>
-      </c>
-      <c r="T10" s="3">
-        <v>3</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+      <c r="S10" s="3"/>
+      <c r="T10" s="3"/>
       <c r="U10" s="3"/>
       <c r="V10" s="3"/>
       <c r="W10" s="3"/>
-      <c r="X10" s="3"/>
-      <c r="Y10" s="3"/>
-      <c r="Z10" s="3"/>
-      <c r="AA10" s="3"/>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B11" s="3">
         <v>4</v>
@@ -1277,47 +1141,35 @@
         <v>4</v>
       </c>
       <c r="J11" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K11" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L11" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M11" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="N11" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O11" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="P11" s="3">
-        <v>2</v>
-      </c>
-      <c r="Q11" s="3">
-        <v>3</v>
-      </c>
-      <c r="R11" s="3">
-        <v>5</v>
-      </c>
-      <c r="S11" s="3">
-        <v>1</v>
-      </c>
-      <c r="T11" s="3">
-        <v>4</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+      <c r="S11" s="3"/>
+      <c r="T11" s="3"/>
       <c r="U11" s="3"/>
       <c r="V11" s="3"/>
       <c r="W11" s="3"/>
-      <c r="X11" s="3"/>
-      <c r="Y11" s="3"/>
-      <c r="Z11" s="3"/>
-      <c r="AA11" s="3"/>
-    </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>4</v>
       </c>
@@ -1346,49 +1198,37 @@
         <v>5</v>
       </c>
       <c r="J12" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K12" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L12" s="3">
         <v>4</v>
       </c>
       <c r="M12" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N12" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="O12" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="P12" s="3">
-        <v>3</v>
-      </c>
-      <c r="Q12" s="3">
-        <v>2</v>
-      </c>
-      <c r="R12" s="3">
-        <v>3</v>
-      </c>
-      <c r="S12" s="3">
-        <v>3</v>
-      </c>
-      <c r="T12" s="3">
-        <v>4</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
+      <c r="S12" s="3"/>
+      <c r="T12" s="3"/>
       <c r="U12" s="3"/>
       <c r="V12" s="3"/>
       <c r="W12" s="3"/>
-      <c r="X12" s="3"/>
-      <c r="Y12" s="3"/>
-      <c r="Z12" s="3"/>
-      <c r="AA12" s="3"/>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B13" s="3">
         <v>4</v>
@@ -1418,7 +1258,7 @@
         <v>4</v>
       </c>
       <c r="K13" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L13" s="3">
         <v>4</v>
@@ -1433,31 +1273,19 @@
         <v>4</v>
       </c>
       <c r="P13" s="3">
-        <v>3</v>
-      </c>
-      <c r="Q13" s="3">
-        <v>4</v>
-      </c>
-      <c r="R13" s="3">
-        <v>4</v>
-      </c>
-      <c r="S13" s="3">
-        <v>4</v>
-      </c>
-      <c r="T13" s="3">
-        <v>4</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
+      <c r="S13" s="3"/>
+      <c r="T13" s="3"/>
       <c r="U13" s="3"/>
       <c r="V13" s="3"/>
       <c r="W13" s="3"/>
-      <c r="X13" s="3"/>
-      <c r="Y13" s="3"/>
-      <c r="Z13" s="3"/>
-      <c r="AA13" s="3"/>
-    </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B14" s="3">
         <v>4</v>
@@ -1484,49 +1312,37 @@
         <v>3</v>
       </c>
       <c r="J14" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K14" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L14" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M14" s="3">
         <v>4</v>
       </c>
       <c r="N14" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O14" s="3">
         <v>4</v>
       </c>
       <c r="P14" s="3">
-        <v>4</v>
-      </c>
-      <c r="Q14" s="3">
-        <v>4</v>
-      </c>
-      <c r="R14" s="3">
-        <v>4</v>
-      </c>
-      <c r="S14" s="3">
-        <v>4</v>
-      </c>
-      <c r="T14" s="3">
-        <v>5</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3"/>
+      <c r="S14" s="3"/>
+      <c r="T14" s="3"/>
       <c r="U14" s="3"/>
       <c r="V14" s="3"/>
       <c r="W14" s="3"/>
-      <c r="X14" s="3"/>
-      <c r="Y14" s="3"/>
-      <c r="Z14" s="3"/>
-      <c r="AA14" s="3"/>
-    </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B15" s="3">
         <v>2</v>
@@ -1553,10 +1369,10 @@
         <v>4</v>
       </c>
       <c r="J15" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K15" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L15" s="3">
         <v>3</v>
@@ -1565,37 +1381,25 @@
         <v>3</v>
       </c>
       <c r="N15" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O15" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P15" s="3">
-        <v>3</v>
-      </c>
-      <c r="Q15" s="3">
-        <v>4</v>
-      </c>
-      <c r="R15" s="3">
-        <v>3</v>
-      </c>
-      <c r="S15" s="3">
-        <v>2</v>
-      </c>
-      <c r="T15" s="3">
-        <v>4</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="3"/>
+      <c r="S15" s="3"/>
+      <c r="T15" s="3"/>
       <c r="U15" s="3"/>
       <c r="V15" s="3"/>
       <c r="W15" s="3"/>
-      <c r="X15" s="3"/>
-      <c r="Y15" s="3"/>
-      <c r="Z15" s="3"/>
-      <c r="AA15" s="3"/>
-    </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B16" s="3">
         <v>3</v>
@@ -1622,10 +1426,10 @@
         <v>4</v>
       </c>
       <c r="J16" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K16" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L16" s="3">
         <v>4</v>
@@ -1634,37 +1438,25 @@
         <v>4</v>
       </c>
       <c r="N16" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O16" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P16" s="3">
-        <v>4</v>
-      </c>
-      <c r="Q16" s="3">
-        <v>3</v>
-      </c>
-      <c r="R16" s="3">
-        <v>4</v>
-      </c>
-      <c r="S16" s="3">
-        <v>3</v>
-      </c>
-      <c r="T16" s="3">
-        <v>5</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="Q16" s="3"/>
+      <c r="R16" s="3"/>
+      <c r="S16" s="3"/>
+      <c r="T16" s="3"/>
       <c r="U16" s="3"/>
       <c r="V16" s="3"/>
       <c r="W16" s="3"/>
-      <c r="X16" s="3"/>
-      <c r="Y16" s="3"/>
-      <c r="Z16" s="3"/>
-      <c r="AA16" s="3"/>
-    </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B17" s="3">
         <v>4</v>
@@ -1694,7 +1486,7 @@
         <v>3</v>
       </c>
       <c r="K17" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L17" s="3">
         <v>4</v>
@@ -1706,34 +1498,22 @@
         <v>4</v>
       </c>
       <c r="O17" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P17" s="3">
-        <v>4</v>
-      </c>
-      <c r="Q17" s="3">
-        <v>4</v>
-      </c>
-      <c r="R17" s="3">
-        <v>4</v>
-      </c>
-      <c r="S17" s="3">
-        <v>4</v>
-      </c>
-      <c r="T17" s="3">
-        <v>5</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="Q17" s="3"/>
+      <c r="R17" s="3"/>
+      <c r="S17" s="3"/>
+      <c r="T17" s="3"/>
       <c r="U17" s="3"/>
       <c r="V17" s="3"/>
       <c r="W17" s="3"/>
-      <c r="X17" s="3"/>
-      <c r="Y17" s="3"/>
-      <c r="Z17" s="3"/>
-      <c r="AA17" s="3"/>
-    </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B18" s="3">
         <v>4</v>
@@ -1760,10 +1540,10 @@
         <v>3</v>
       </c>
       <c r="J18" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K18" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L18" s="3">
         <v>4</v>
@@ -1775,32 +1555,20 @@
         <v>4</v>
       </c>
       <c r="O18" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P18" s="3">
-        <v>4</v>
-      </c>
-      <c r="Q18" s="3">
-        <v>4</v>
-      </c>
-      <c r="R18" s="3">
-        <v>4</v>
-      </c>
-      <c r="S18" s="3">
-        <v>3</v>
-      </c>
-      <c r="T18" s="3">
-        <v>5</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="Q18" s="3"/>
+      <c r="R18" s="3"/>
+      <c r="S18" s="3"/>
+      <c r="T18" s="3"/>
       <c r="U18" s="3"/>
       <c r="V18" s="3"/>
       <c r="W18" s="3"/>
-      <c r="X18" s="3"/>
-      <c r="Y18" s="3"/>
-      <c r="Z18" s="3"/>
-      <c r="AA18" s="3"/>
-    </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>5</v>
       </c>
@@ -1829,47 +1597,35 @@
         <v>4</v>
       </c>
       <c r="J19" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K19" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L19" s="3">
         <v>5</v>
       </c>
       <c r="M19" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="N19" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O19" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P19" s="3">
         <v>5</v>
       </c>
-      <c r="Q19" s="3">
-        <v>4</v>
-      </c>
-      <c r="R19" s="3">
-        <v>5</v>
-      </c>
-      <c r="S19" s="3">
-        <v>4</v>
-      </c>
-      <c r="T19" s="3">
-        <v>5</v>
-      </c>
+      <c r="Q19" s="3"/>
+      <c r="R19" s="3"/>
+      <c r="S19" s="3"/>
+      <c r="T19" s="3"/>
       <c r="U19" s="3"/>
       <c r="V19" s="3"/>
       <c r="W19" s="3"/>
-      <c r="X19" s="3"/>
-      <c r="Y19" s="3"/>
-      <c r="Z19" s="3"/>
-      <c r="AA19" s="3"/>
-    </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>6</v>
       </c>
@@ -1898,7 +1654,7 @@
         <v>3</v>
       </c>
       <c r="J20" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K20" s="3">
         <v>4</v>
@@ -1913,33 +1669,21 @@
         <v>4</v>
       </c>
       <c r="O20" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P20" s="3">
-        <v>4</v>
-      </c>
-      <c r="Q20" s="3">
-        <v>4</v>
-      </c>
-      <c r="R20" s="3">
-        <v>4</v>
-      </c>
-      <c r="S20" s="3">
-        <v>4</v>
-      </c>
-      <c r="T20" s="3">
-        <v>5</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="Q20" s="3"/>
+      <c r="R20" s="3"/>
+      <c r="S20" s="3"/>
+      <c r="T20" s="3"/>
       <c r="U20" s="3"/>
       <c r="V20" s="3"/>
       <c r="W20" s="3"/>
       <c r="X20" s="3"/>
-      <c r="Y20" s="3"/>
-      <c r="Z20" s="3"/>
-      <c r="AA20" s="3"/>
-      <c r="AB20" s="3"/>
-    </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>7</v>
       </c>
@@ -1971,39 +1715,27 @@
         <v>2</v>
       </c>
       <c r="K21" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L21" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M21" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N21" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O21" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P21" s="3">
-        <v>3</v>
-      </c>
-      <c r="Q21" s="3">
-        <v>3</v>
-      </c>
-      <c r="R21" s="3">
-        <v>4</v>
-      </c>
-      <c r="S21" s="3">
-        <v>2</v>
-      </c>
-      <c r="T21" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B22" s="3">
         <v>5</v>
@@ -2030,10 +1762,10 @@
         <v>4</v>
       </c>
       <c r="J22" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K22" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L22" s="3">
         <v>4</v>
@@ -2048,22 +1780,10 @@
         <v>4</v>
       </c>
       <c r="P22" s="3">
-        <v>4</v>
-      </c>
-      <c r="Q22" s="3">
-        <v>4</v>
-      </c>
-      <c r="R22" s="3">
-        <v>4</v>
-      </c>
-      <c r="S22" s="3">
-        <v>4</v>
-      </c>
-      <c r="T22" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>8</v>
       </c>
@@ -2095,16 +1815,16 @@
         <v>3</v>
       </c>
       <c r="K23" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L23" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M23" s="3">
         <v>4</v>
       </c>
       <c r="N23" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O23" s="3">
         <v>4</v>
@@ -2112,20 +1832,8 @@
       <c r="P23" s="3">
         <v>4</v>
       </c>
-      <c r="Q23" s="3">
-        <v>4</v>
-      </c>
-      <c r="R23" s="3">
-        <v>4</v>
-      </c>
-      <c r="S23" s="3">
-        <v>4</v>
-      </c>
-      <c r="T23" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>9</v>
       </c>
@@ -2154,40 +1862,28 @@
         <v>4</v>
       </c>
       <c r="J24" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K24" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L24" s="3">
         <v>3</v>
       </c>
       <c r="M24" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="N24" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O24" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P24" s="3">
         <v>5</v>
       </c>
-      <c r="Q24" s="3">
-        <v>4</v>
-      </c>
-      <c r="R24" s="3">
-        <v>3</v>
-      </c>
-      <c r="S24" s="3">
-        <v>3</v>
-      </c>
-      <c r="T24" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>10</v>
       </c>
@@ -2216,19 +1912,19 @@
         <v>4</v>
       </c>
       <c r="J25" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K25" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="L25" s="3">
         <v>4</v>
       </c>
       <c r="M25" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="N25" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="O25" s="3">
         <v>4</v>
@@ -2236,20 +1932,8 @@
       <c r="P25" s="3">
         <v>5</v>
       </c>
-      <c r="Q25" s="3">
-        <v>1</v>
-      </c>
-      <c r="R25" s="3">
-        <v>4</v>
-      </c>
-      <c r="S25" s="3">
-        <v>3</v>
-      </c>
-      <c r="T25" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>11</v>
       </c>
@@ -2278,7 +1962,7 @@
         <v>4</v>
       </c>
       <c r="J26" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K26" s="3">
         <v>4</v>
@@ -2293,25 +1977,13 @@
         <v>4</v>
       </c>
       <c r="O26" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P26" s="3">
-        <v>4</v>
-      </c>
-      <c r="Q26" s="3">
-        <v>4</v>
-      </c>
-      <c r="R26" s="3">
-        <v>4</v>
-      </c>
-      <c r="S26" s="3">
-        <v>3</v>
-      </c>
-      <c r="T26" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>12</v>
       </c>
@@ -2340,36 +2012,24 @@
         <v>2</v>
       </c>
       <c r="J27" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K27" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L27" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="M27" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="N27" s="3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="O27" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="P27" s="3">
-        <v>2</v>
-      </c>
-      <c r="Q27" s="3">
-        <v>2</v>
-      </c>
-      <c r="R27" s="3">
-        <v>5</v>
-      </c>
-      <c r="S27" s="3">
-        <v>1</v>
-      </c>
-      <c r="T27" s="3">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Final version of clustering
</commit_message>
<xml_diff>
--- a/DataVisualization.xlsx
+++ b/DataVisualization.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chakotay Incorvaia\dev2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60C5F49D-9523-48ED-A63A-86E5A38D3636}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95596273-62E3-409B-BDD6-27EA640A449D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{CCE0E44F-0ABA-4097-A493-E6A10D57D926}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{CCE0E44F-0ABA-4097-A493-E6A10D57D926}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -518,7 +518,7 @@
   <dimension ref="A1:X27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,7 +604,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" s="2">
         <v>5</v>
@@ -718,7 +718,7 @@
         <v>41</v>
       </c>
       <c r="B4" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" s="2">
         <v>5</v>
@@ -1060,7 +1060,7 @@
         <v>3</v>
       </c>
       <c r="B10" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C10" s="3">
         <v>4</v>

</xml_diff>

<commit_message>
Simple Visualization of Procedures
</commit_message>
<xml_diff>
--- a/DataVisualization.xlsx
+++ b/DataVisualization.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chakotay Incorvaia\dev2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95596273-62E3-409B-BDD6-27EA640A449D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{306E8482-1F57-4AA1-A4A0-0401D6105843}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{CCE0E44F-0ABA-4097-A493-E6A10D57D926}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{CCE0E44F-0ABA-4097-A493-E6A10D57D926}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="QualitySheet" sheetId="1" r:id="rId1"/>
+    <sheet name="PhaseSheet" sheetId="2" r:id="rId2"/>
+    <sheet name="SequenceSheet" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="59">
   <si>
     <t>Accuracy</t>
   </si>
@@ -159,6 +161,57 @@
   </si>
   <si>
     <t>Understandability</t>
+  </si>
+  <si>
+    <t>Procedures</t>
+  </si>
+  <si>
+    <t>Preliminary Preflight Procedure</t>
+  </si>
+  <si>
+    <t>CDU Preflight Procedure</t>
+  </si>
+  <si>
+    <t>Preflight Procedure</t>
+  </si>
+  <si>
+    <t>Before Start Procedure</t>
+  </si>
+  <si>
+    <t>Pushback or Towing Procedure</t>
+  </si>
+  <si>
+    <t>Engine Start Procedure</t>
+  </si>
+  <si>
+    <t>Before Taxi Procedure</t>
+  </si>
+  <si>
+    <t>Takeoff Procedure</t>
+  </si>
+  <si>
+    <t>Climb and Cruise Procedure</t>
+  </si>
+  <si>
+    <t>Descent Procedure</t>
+  </si>
+  <si>
+    <t>Approach Procedure</t>
+  </si>
+  <si>
+    <t>Landing Procedure</t>
+  </si>
+  <si>
+    <t>Landing Roll Procedure</t>
+  </si>
+  <si>
+    <t>After Landing Procedure</t>
+  </si>
+  <si>
+    <t>Instrument</t>
+  </si>
+  <si>
+    <t>Sequence</t>
   </si>
 </sst>
 </file>
@@ -194,13 +247,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -515,10 +571,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49A2CE25-1FB0-46F3-A95B-A7BCC2B1E34D}">
-  <dimension ref="A1:X27"/>
+  <dimension ref="A1:X28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29:XFD29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2033,8 +2089,970 @@
         <v>5</v>
       </c>
     </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="3"/>
+      <c r="O28" s="3"/>
+      <c r="P28" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{407E7872-AEB2-439A-AA22-2EFACC4ADFCE}">
+  <dimension ref="A1:P15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4">
+        <v>1</v>
+      </c>
+      <c r="P4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>1</v>
+      </c>
+      <c r="P7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>1</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>1</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>1</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F027EA97-39C6-4A00-847A-7E78910072DF}">
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" customWidth="1"/>
+    <col min="4" max="4" width="11" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" customWidth="1"/>
+    <col min="9" max="9" width="8.7109375" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.85546875" customWidth="1"/>
+    <col min="12" max="12" width="18.28515625" customWidth="1"/>
+    <col min="13" max="13" width="14" customWidth="1"/>
+    <col min="14" max="14" width="11.42578125" customWidth="1"/>
+    <col min="15" max="15" width="18.28515625" customWidth="1"/>
+    <col min="16" max="16" width="16.140625" customWidth="1"/>
+    <col min="17" max="17" width="20" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18.28515625" customWidth="1"/>
+    <col min="23" max="23" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>